<commit_message>
solved 2 more questions
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t xml:space="preserve">Question Name</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/best-time-to-buy-and-sell-stock/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO AGAIN</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,6 +222,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,10 +314,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="F2:G5 E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -395,21 +406,21 @@
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -426,23 +437,70 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C200" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B201" s="4"/>
+      <c r="C201" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F201" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G201" s="4"/>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B202" s="7"/>
+      <c r="C202" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D202" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F202" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G202" s="7"/>
+      <c r="H202" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -466,7 +524,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F2:G5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -489,7 +547,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F2:G5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>